<commit_message>
updating bands to DiMascolo25 band edges
</commit_message>
<xml_diff>
--- a/instrument_definition_inputs.xlsx
+++ b/instrument_definition_inputs.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbryan/Documents/atlast-telescope/sens_calc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanb\Documents\atlast\sens_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348916C3-97DB-7648-9F50-48BCA372F3D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3F0F00-6BE3-4D27-B73C-42697A36EBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27340" yWindow="-10200" windowWidth="21240" windowHeight="11200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="72468" yWindow="3624" windowWidth="19272" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -23,6 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -365,19 +371,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,54 +397,54 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="B2">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="B3">
-        <v>170</v>
+        <v>117</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
-        <v>195</v>
+        <v>120</v>
       </c>
       <c r="B4">
-        <v>245</v>
+        <v>182</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
-        <v>245</v>
+        <v>183</v>
       </c>
       <c r="B5">
-        <v>310</v>
+        <v>252</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -447,74 +453,88 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
-        <v>335</v>
+        <v>252</v>
       </c>
       <c r="B6">
-        <v>365</v>
+        <v>325</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D6">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>325</v>
+      </c>
+      <c r="B7">
         <v>375</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>390</v>
-      </c>
-      <c r="B7">
-        <v>420</v>
-      </c>
       <c r="C7">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>375</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
-        <v>625</v>
+        <v>384</v>
       </c>
       <c r="B8">
-        <v>710</v>
+        <v>422</v>
       </c>
       <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>595</v>
+      </c>
+      <c r="B9">
+        <v>713</v>
+      </c>
+      <c r="C9">
         <v>10</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>640</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>845</v>
-      </c>
-      <c r="B9">
-        <v>900</v>
-      </c>
-      <c r="C9">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>786</v>
+      </c>
+      <c r="B10">
+        <v>905</v>
+      </c>
+      <c r="C10">
         <v>6</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>870</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="C10">
-        <f>SUM(C2,C4,C6,C8,C9)</f>
+      <c r="C11">
+        <f>SUM(C2,C3,C5,C7,C9,C10)</f>
         <v>50</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>